<commit_message>
change the default of pvalues_weight to TRUE
</commit_message>
<xml_diff>
--- a/inst/extdata/LDL_C.xlsx
+++ b/inst/extdata/LDL_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/yzh10_iu_edu/Documents/research/nuMoM2b/whole_sequencing/mr.carv/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{EB338793-E911-CF44-9B38-94A76EF1FAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E3D53E5-FE45-0443-A1F1-B73002164951}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{EB338793-E911-CF44-9B38-94A76EF1FAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FDCB031-C145-3941-8751-3531E83D0FDC}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2720" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{8CF3AADF-3B51-1B4F-985A-713C56632C1E}"/>
+    <workbookView xWindow="5400" yWindow="780" windowWidth="30240" windowHeight="18880" xr2:uid="{8CF3AADF-3B51-1B4F-985A-713C56632C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="indv_effect" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="506">
   <si>
     <t>A</t>
   </si>
@@ -1404,9 +1404,6 @@
   </si>
   <si>
     <t>rs138994584</t>
-  </si>
-  <si>
-    <t>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000156554505296365</t>
   </si>
   <si>
     <t>rs72654441</t>
@@ -2372,13 +2369,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507F472E-772F-E949-B612-5FED0D7A26C2}">
   <dimension ref="A1:L339"/>
   <sheetViews>
-    <sheetView topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L339"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="G288" sqref="G288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" customWidth="1"/>
   </cols>
@@ -13683,8 +13681,8 @@
       <c r="G300" s="3">
         <v>0.37594864250705301</v>
       </c>
-      <c r="H300" s="4" t="s">
-        <v>455</v>
+      <c r="H300" s="4">
+        <v>1.5655450529636499E-302</v>
       </c>
       <c r="I300" s="3">
         <v>0.112378597259521</v>
@@ -13751,7 +13749,7 @@
         <v>10</v>
       </c>
       <c r="E302" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F302" s="3">
         <v>-20.123173258206201</v>
@@ -13789,7 +13787,7 @@
         <v>6</v>
       </c>
       <c r="E303" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F303" s="3">
         <v>-2.7092588955619101</v>
@@ -13827,7 +13825,7 @@
         <v>6</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F304" s="3">
         <v>-19.038618671961501</v>
@@ -14283,7 +14281,7 @@
         <v>6</v>
       </c>
       <c r="E316" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F316" s="3">
         <v>-9.9816140269214504</v>
@@ -14435,7 +14433,7 @@
         <v>10</v>
       </c>
       <c r="E320" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F320" s="3">
         <v>-1.6441450557324899</v>
@@ -14473,7 +14471,7 @@
         <v>10</v>
       </c>
       <c r="E321" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F321" s="3">
         <v>-1.9158291395856399</v>
@@ -14625,7 +14623,7 @@
         <v>1</v>
       </c>
       <c r="E325" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F325" s="3">
         <v>-15.9191528507369</v>
@@ -14663,7 +14661,7 @@
         <v>6</v>
       </c>
       <c r="E326" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F326" s="3">
         <v>-20.964948571041301</v>
@@ -14739,7 +14737,7 @@
         <v>1</v>
       </c>
       <c r="E328" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F328" s="3">
         <v>-16.405935485318999</v>
@@ -14815,7 +14813,7 @@
         <v>6</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F330" s="3">
         <v>-10.6719938708319</v>
@@ -14833,7 +14831,7 @@
         <v>14</v>
       </c>
       <c r="K330" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L330" s="6" t="s">
         <v>5</v>
@@ -14891,7 +14889,7 @@
         <v>6</v>
       </c>
       <c r="E332" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F332" s="3">
         <v>-7.6597054184176301</v>
@@ -14909,7 +14907,7 @@
         <v>14</v>
       </c>
       <c r="K332" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L332" s="6" t="s">
         <v>5</v>
@@ -15003,7 +15001,7 @@
         <v>10</v>
       </c>
       <c r="E335" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F335" s="3">
         <v>1.47530948282767</v>
@@ -15021,7 +15019,7 @@
         <v>8</v>
       </c>
       <c r="K335" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L335" s="6" t="s">
         <v>5</v>
@@ -15079,7 +15077,7 @@
         <v>6</v>
       </c>
       <c r="E337" s="43" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F337" s="44">
         <v>-16.086004369189901</v>
@@ -15115,7 +15113,7 @@
         <v>1</v>
       </c>
       <c r="E338" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F338" s="3">
         <v>-12.4386743947619</v>
@@ -15151,7 +15149,7 @@
         <v>6</v>
       </c>
       <c r="E339" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F339" s="3">
         <v>-1.5682834501227201</v>
@@ -15253,10 +15251,10 @@
         <v>185</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F2" s="13">
         <v>221</v>
@@ -15300,10 +15298,10 @@
         <v>185</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F3" s="20">
         <v>203</v>
@@ -15350,7 +15348,7 @@
         <v>164</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F4" s="20">
         <v>343</v>
@@ -15488,7 +15486,7 @@
         <v>185</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>168</v>
@@ -15535,7 +15533,7 @@
         <v>185</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>163</v>
@@ -15582,7 +15580,7 @@
         <v>185</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>169</v>
@@ -15676,7 +15674,7 @@
         <v>185</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>163</v>
@@ -15723,7 +15721,7 @@
         <v>185</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>163</v>
@@ -15958,7 +15956,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>163</v>
@@ -16005,7 +16003,7 @@
         <v>185</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E18" s="27" t="s">
         <v>163</v>
@@ -16117,7 +16115,7 @@
         <v>185</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>163</v>
@@ -16164,7 +16162,7 @@
         <v>185</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>163</v>
@@ -16211,7 +16209,7 @@
         <v>185</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>163</v>
@@ -16258,7 +16256,7 @@
         <v>185</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>186</v>
@@ -16305,7 +16303,7 @@
         <v>185</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>186</v>
@@ -16350,7 +16348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65817AE-EFB2-3149-A03E-023FCF44018F}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
@@ -16362,19 +16360,19 @@
         <v>154</v>
       </c>
       <c r="B1" s="50" t="s">
+        <v>479</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>480</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>481</v>
       </c>
       <c r="D1" s="51" t="s">
         <v>175</v>
       </c>
       <c r="E1" s="52" t="s">
+        <v>481</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>482</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>483</v>
       </c>
       <c r="G1" s="53" t="s">
         <v>342</v>
@@ -16412,7 +16410,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G2" s="68">
         <v>1.079</v>
@@ -16450,7 +16448,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G3" s="69">
         <v>1.133</v>
@@ -16488,7 +16486,7 @@
         <v>167</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G4" s="69">
         <v>-1.5940000000000001</v>
@@ -16526,7 +16524,7 @@
         <v>167</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G5" s="69">
         <v>-0.96499999999999997</v>
@@ -16564,7 +16562,7 @@
         <v>167</v>
       </c>
       <c r="F6" s="64" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G6" s="69">
         <v>-0.84599999999999997</v>
@@ -16602,7 +16600,7 @@
         <v>167</v>
       </c>
       <c r="F7" s="64" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G7" s="69">
         <v>7.8E-2</v>
@@ -16640,7 +16638,7 @@
         <v>285</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G8" s="69">
         <v>-3.6749999999999998</v>
@@ -16678,7 +16676,7 @@
         <v>167</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G9" s="69">
         <v>0.80600000000000005</v>
@@ -16716,7 +16714,7 @@
         <v>285</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G10" s="69">
         <v>-4.1630000000000003</v>
@@ -16751,7 +16749,7 @@
         <v>292</v>
       </c>
       <c r="E11" s="65" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F11" s="57" t="s">
         <v>163</v>
@@ -16792,7 +16790,7 @@
         <v>310</v>
       </c>
       <c r="F12" s="67" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G12" s="70">
         <v>0.20599999999999999</v>
@@ -16830,7 +16828,7 @@
         <v>45</v>
       </c>
       <c r="F13" s="55" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G13" s="84">
         <v>20.0247796115755</v>
@@ -16868,7 +16866,7 @@
         <v>45</v>
       </c>
       <c r="F14" s="57" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G14" s="86">
         <v>10.5340295244686</v>
@@ -16906,7 +16904,7 @@
         <v>167</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G15" s="86">
         <v>-6.0423180695721301</v>
@@ -16944,7 +16942,7 @@
         <v>45</v>
       </c>
       <c r="F16" s="57" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G16" s="86">
         <v>8.54962241461606</v>
@@ -16982,7 +16980,7 @@
         <v>167</v>
       </c>
       <c r="F17" s="57" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G17" s="86">
         <v>-2.4949373374766002</v>
@@ -17020,7 +17018,7 @@
         <v>45</v>
       </c>
       <c r="F18" s="57" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G18" s="86">
         <v>17.5009942371161</v>
@@ -17058,7 +17056,7 @@
         <v>167</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G19" s="86">
         <v>-2.13866459713556</v>
@@ -17096,7 +17094,7 @@
         <v>167</v>
       </c>
       <c r="F20" s="57" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G20" s="86">
         <v>-1.69410081805676</v>
@@ -17134,7 +17132,7 @@
         <v>285</v>
       </c>
       <c r="F21" s="82" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G21" s="86">
         <v>-4.2064582405028004</v>
@@ -17172,7 +17170,7 @@
         <v>45</v>
       </c>
       <c r="F22" s="57" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G22" s="86">
         <v>12.3670944593001</v>
@@ -17210,7 +17208,7 @@
         <v>45</v>
       </c>
       <c r="F23" s="57" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G23" s="86">
         <v>11.5091847363411</v>
@@ -17248,7 +17246,7 @@
         <v>285</v>
       </c>
       <c r="F24" s="82" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G24" s="86">
         <v>-4.1416573339641598</v>
@@ -17283,7 +17281,7 @@
         <v>300</v>
       </c>
       <c r="E25" s="81" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F25" s="57" t="s">
         <v>163</v>
@@ -17324,7 +17322,7 @@
         <v>167</v>
       </c>
       <c r="F26" s="57" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G26" s="86">
         <v>1.1369109319513699</v>
@@ -17359,7 +17357,7 @@
         <v>180</v>
       </c>
       <c r="E27" s="81" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F27" s="57" t="s">
         <v>163</v>
@@ -17400,7 +17398,7 @@
         <v>310</v>
       </c>
       <c r="F28" s="57" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G28" s="86">
         <v>0.29896794730308401</v>
@@ -17438,7 +17436,7 @@
         <v>167</v>
       </c>
       <c r="F29" s="57" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G29" s="86">
         <v>-2.8175610802823398E-2</v>
@@ -17473,7 +17471,7 @@
         <v>290</v>
       </c>
       <c r="E30" s="81" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F30" s="57" t="s">
         <v>163</v>
@@ -17511,7 +17509,7 @@
         <v>50</v>
       </c>
       <c r="E31" s="83" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F31" s="59" t="s">
         <v>163</v>

</xml_diff>